<commit_message>
get dhamma.org "Other" from other_course in central db
</commit_message>
<xml_diff>
--- a/data/course_type_map.xlsx
+++ b/data/course_type_map.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t xml:space="preserve">raw_course_type</t>
   </si>
@@ -28,9 +28,6 @@
     <t xml:space="preserve">period_type</t>
   </si>
   <si>
-    <t xml:space="preserve">course_type</t>
-  </si>
-  <si>
     <t xml:space="preserve">10-Day</t>
   </si>
   <si>
@@ -47,15 +44,6 @@
   </si>
   <si>
     <t xml:space="preserve">Children / teens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trust WE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">|TRUST MEETING|</t>
   </si>
   <si>
     <t xml:space="preserve">3-Day</t>
@@ -289,17 +277,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="30.74"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -309,91 +296,77 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>